<commit_message>
Erro de expansão arrumado, agora a interface se ajusta conforme o tamanho da tela
</commit_message>
<xml_diff>
--- a/estoque.xlsx
+++ b/estoque.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -547,7 +547,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -556,7 +556,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>19/09/2025 20:42</t>
+          <t>21/10/2025 17:57</t>
         </is>
       </c>
     </row>
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -606,7 +606,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>19/09/2025 14:51</t>
+          <t>21/10/2025 19:51</t>
         </is>
       </c>
     </row>
@@ -797,7 +797,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -806,32 +806,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>25/09/2025 23:08</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Cano T</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>ID_13</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>4</v>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>19/09/2025 20:43</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>25/09/2025 23:17</t>
+          <t>21/10/2025 19:58</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Erro de expansão arrumado, agora a interface se ajusta conforme o tamanho da tela adcionado função de senha para edição adcionado edição de imagem troca de formulario
</commit_message>
<xml_diff>
--- a/estoque.xlsx
+++ b/estoque.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Estoque" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Removidos" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,10 +452,15 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Preco</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Data_Criacao</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Data_Alteracao</t>
         </is>
@@ -463,232 +469,259 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Cano L</t>
+          <t>Argamassa 20kg</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ID_2</t>
+          <t>ID_1</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>19</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>19/09/2025 14:55</t>
-        </is>
+        <v>16</v>
+      </c>
+      <c r="D2" t="n">
+        <v>50</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>19/09/2025 20:35</t>
+          <t>21/10/2025 22:24</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:55</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Cano Las</t>
+          <t>Betoneira</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ID_4</t>
+          <t>ID_2</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>19/09/2025 19:51</t>
-        </is>
+        <v>5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>4000</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>19/09/2025 20:49</t>
+          <t>21/10/2025 22:25</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>21/10/2025 23:49</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Cano y</t>
+          <t>Bucha 12 mm</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ID_5</t>
+          <t>ID_3</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>19/09/2025 19:51</t>
-        </is>
+        <v>340</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.13</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>25/09/2025 23:07</t>
+          <t>21/10/2025 22:26</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:26</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Cano y</t>
+          <t>bucha 6mm</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ID_6</t>
+          <t>ID_4</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>32</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>19/09/2025 19:51</t>
-        </is>
+        <v>274</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.02</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>21/10/2025 17:57</t>
+          <t>21/10/2025 22:27</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:27</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Cano L</t>
+          <t>Bucha 8mm</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ID_7</t>
+          <t>ID_5</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>19/09/2025 19:51</t>
-        </is>
+        <v>167</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.1</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>19/09/2025 20:42</t>
+          <t>21/10/2025 22:28</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:28</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Cano i</t>
+          <t>buxa 10mm</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ID_1</t>
+          <t>ID_6</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>19/09/2025 14:51</t>
-        </is>
+        <v>190</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.15</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>21/10/2025 19:51</t>
+          <t>21/10/2025 22:28</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:28</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Cano i</t>
+          <t>cimento 20kg</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ID_8</t>
+          <t>ID_7</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>15</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>19/09/2025 19:57</t>
-        </is>
+        <v>25</v>
+      </c>
+      <c r="D8" t="n">
+        <v>406.9</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>25/09/2025 23:16</t>
+          <t>21/10/2025 22:29</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:56</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Cano L</t>
+          <t>cano Iuva</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ID_9</t>
+          <t>ID_8</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>22</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>19/09/2025 20:03</t>
-        </is>
+        <v>23</v>
+      </c>
+      <c r="D9" t="n">
+        <v>9.470000000000001</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>19/09/2025 20:44</t>
+          <t>21/10/2025 22:32</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>21/10/2025 23:51</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Cano T</t>
+          <t>Tubo Joelho</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ID_3</t>
+          <t>ID_9</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>111</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>19/09/2025 14:55</t>
-        </is>
+        <v>43</v>
+      </c>
+      <c r="D10" t="n">
+        <v>5</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>19/09/2025 20:22</t>
+          <t>21/10/2025 22:33</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>21/10/2025 23:41</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Cano I</t>
+          <t>Tubo tee</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -697,23 +730,26 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>14</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>19/09/2025 20:43</t>
-        </is>
+        <v>44</v>
+      </c>
+      <c r="D11" t="n">
+        <v>5.24</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>19/09/2025 20:43</t>
+          <t>21/10/2025 22:34</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:34</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Cano y</t>
+          <t>tubo y</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -722,23 +758,26 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>15</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>19/09/2025 20:43</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="D12" t="n">
+        <v>9.199999999999999</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>25/09/2025 23:08</t>
+          <t>21/10/2025 22:36</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:36</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Cano L</t>
+          <t>parafuso 6mm</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -747,66 +786,636 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>197</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>19/09/2025 20:43</t>
-        </is>
+        <v>154</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.27</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>25/09/2025 23:16</t>
+          <t>21/10/2025 22:36</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:36</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>Prego</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ID_13</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>562</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:38</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:38</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Nome</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Quantidade</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Preco</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Data_Criacao</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Data_Alteracao</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Data_Remocao</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Cano novo</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ID_15</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>18</v>
+      </c>
+      <c r="D2" t="n">
+        <v>23</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:16</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:17</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Cabi Y</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ID_14</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>16</v>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>25/09/2025 23:08</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>21/10/2025 19:58</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>Cano T</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ID_13</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>7</v>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>25/09/2025 23:08</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>25/09/2025 23:08</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Cano L</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ID_2</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>20</v>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>19/09/2025 14:55</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:17</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Cano Las</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ID_4</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>19/09/2025 19:51</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>19/09/2025 20:49</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Cano y</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ID_5</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>4</v>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>19/09/2025 19:51</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>25/09/2025 23:07</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Cano y</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ID_6</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>32</v>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>19/09/2025 19:51</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>21/10/2025 17:57</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Cano L</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ID_7</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>17</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>19/09/2025 19:51</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>19/09/2025 20:42</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Cano i</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ID_1</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>35</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>19/09/2025 14:51</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>21/10/2025 19:51</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Cano i</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ID_8</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>15</v>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>19/09/2025 19:57</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>25/09/2025 23:16</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Cano L</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ID_9</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>22</v>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>19/09/2025 20:03</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>19/09/2025 20:44</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Cano T</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ID_3</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>111</v>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>19/09/2025 14:55</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>19/09/2025 20:22</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Cano I</t>
+        </is>
+      </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ID_13</t>
+          <t>ID_10</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>7</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>25/09/2025 23:08</t>
-        </is>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr">
         <is>
-          <t>25/09/2025 23:08</t>
+          <t>19/09/2025 20:43</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>19/09/2025 20:43</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:17</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Cabi Y</t>
+          <t>Cano y</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>ID_11</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>15</v>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>19/09/2025 20:43</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>25/09/2025 23:08</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Cano L</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ID_12</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>197</v>
+      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>19/09/2025 20:43</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>25/09/2025 23:16</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Gugu</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
           <t>ID_14</t>
         </is>
       </c>
-      <c r="C15" t="n">
-        <v>16</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>25/09/2025 23:08</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>21/10/2025 19:58</t>
+      <c r="C17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" t="n">
+        <v>9999</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>21/10/2025 23:41</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>21/10/2025 23:41</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>21/10/2025 23:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>maquita</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>ID_15</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>13</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2500</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>21/10/2025 23:42</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>21/10/2025 23:42</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>21/10/2025 23:51</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Novo layout de pagina Nova função de categoria Nova função de pesquisa
</commit_message>
<xml_diff>
--- a/estoque.xlsx
+++ b/estoque.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Estoque" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Removidos" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Categorias" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,10 +458,15 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Categoria</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Data_Criacao</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Data_Alteracao</t>
         </is>
@@ -485,12 +491,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>cimento</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>21/10/2025 22:24</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>21/10/2025 22:55</t>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>29/10/2025 21:22</t>
         </is>
       </c>
     </row>
@@ -513,12 +524,17 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
+          <t>maquinas</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>21/10/2025 22:25</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>21/10/2025 23:49</t>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>29/10/2025 21:24</t>
         </is>
       </c>
     </row>
@@ -541,12 +557,17 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
+          <t>bucha</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
           <t>21/10/2025 22:26</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>21/10/2025 22:26</t>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>29/10/2025 21:21</t>
         </is>
       </c>
     </row>
@@ -569,12 +590,17 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
+          <t>bucha</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>21/10/2025 22:27</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>21/10/2025 22:27</t>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>29/10/2025 21:21</t>
         </is>
       </c>
     </row>
@@ -597,12 +623,17 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
+          <t>bucha</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
           <t>21/10/2025 22:28</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>21/10/2025 22:28</t>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>29/10/2025 21:21</t>
         </is>
       </c>
     </row>
@@ -625,215 +656,255 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
+          <t>bucha</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
           <t>21/10/2025 22:28</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>21/10/2025 22:28</t>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>29/10/2025 21:21</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>cimento 20kg</t>
+          <t>cano Iuva</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ID_7</t>
+          <t>ID_8</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D8" t="n">
-        <v>406.9</v>
+        <v>9.470000000000001</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>21/10/2025 22:29</t>
+          <t>canos</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>21/10/2025 22:56</t>
+          <t>21/10/2025 22:32</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>29/10/2025 21:22</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>cano Iuva</t>
+          <t>Tubo Joelho</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ID_8</t>
+          <t>ID_9</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="D9" t="n">
-        <v>9.470000000000001</v>
+        <v>5</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>21/10/2025 22:32</t>
+          <t>canos</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>23/10/2025 23:18</t>
+          <t>21/10/2025 22:33</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>29/10/2025 21:22</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Tubo Joelho</t>
+          <t>Tubo tee</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ID_9</t>
+          <t>ID_10</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D10" t="n">
-        <v>5</v>
+        <v>5.24</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>21/10/2025 22:33</t>
+          <t>canos</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>21/10/2025 23:41</t>
+          <t>21/10/2025 22:34</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>29/10/2025 21:22</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Tubo tee</t>
+          <t>tubo y</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ID_10</t>
+          <t>ID_11</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>5.24</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>21/10/2025 22:34</t>
+          <t>canos</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>21/10/2025 22:34</t>
+          <t>21/10/2025 22:36</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>29/10/2025 21:22</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>tubo y</t>
+          <t>parafuso 6mm</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ID_11</t>
+          <t>ID_12</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>154</v>
       </c>
       <c r="D12" t="n">
-        <v>9.199999999999999</v>
+        <v>0.27</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
+          <t>parafusos</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
           <t>21/10/2025 22:36</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>21/10/2025 22:36</t>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>29/10/2025 21:23</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>parafuso 6mm</t>
+          <t>Prego</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ID_12</t>
+          <t>ID_13</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>154</v>
+        <v>562</v>
       </c>
       <c r="D13" t="n">
-        <v>0.27</v>
+        <v>0.02</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>21/10/2025 22:36</t>
+          <t>prego</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>21/10/2025 22:36</t>
+          <t>21/10/2025 22:38</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>29/10/2025 21:23</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Prego</t>
+          <t>cimento 20 kg</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ID_13</t>
+          <t>ID_15</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>562</v>
+        <v>15</v>
       </c>
       <c r="D14" t="n">
-        <v>0.02</v>
+        <v>13</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>21/10/2025 22:38</t>
+          <t>cimento</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>21/10/2025 22:38</t>
+          <t>29/10/2025 20:12</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>29/10/2025 20:12</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>gugu</t>
+          <t>maquita</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -845,16 +916,54 @@
         <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>12</v>
+        <v>3000</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>23/10/2025 23:59</t>
+          <t>maquinas</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>23/10/2025 23:59</t>
+          <t>29/10/2025 21:35</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>29/10/2025 21:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>gugu</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ID_15</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" t="n">
+        <v>9999</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>gugu</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>29/10/2025 21:37</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>29/10/2025 21:38</t>
         </is>
       </c>
     </row>
@@ -869,7 +978,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -900,15 +1009,20 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Categoria</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Data_Criacao</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Data_Alteracao</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Data_Remocao</t>
         </is>
@@ -931,15 +1045,20 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
+          <t>Sem Categoria</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>25/09/2025 23:08</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>21/10/2025 19:58</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>21/10/2025 22:17</t>
         </is>
@@ -962,15 +1081,20 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
+          <t>Sem Categoria</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>25/09/2025 23:08</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>25/09/2025 23:08</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>21/10/2025 22:17</t>
         </is>
@@ -993,15 +1117,20 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
+          <t>Sem Categoria</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
           <t>19/09/2025 14:55</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>21/10/2025 22:17</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>21/10/2025 22:17</t>
         </is>
@@ -1024,15 +1153,20 @@
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
+          <t>Sem Categoria</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>19/09/2025 19:51</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>19/09/2025 20:49</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>21/10/2025 22:17</t>
         </is>
@@ -1055,15 +1189,20 @@
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
+          <t>Sem Categoria</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
           <t>19/09/2025 19:51</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>25/09/2025 23:07</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>21/10/2025 22:17</t>
         </is>
@@ -1086,15 +1225,20 @@
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
+          <t>Sem Categoria</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
           <t>19/09/2025 19:51</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>21/10/2025 17:57</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>21/10/2025 22:17</t>
         </is>
@@ -1117,15 +1261,20 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
+          <t>Sem Categoria</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
           <t>19/09/2025 19:51</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>19/09/2025 20:42</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>21/10/2025 22:17</t>
         </is>
@@ -1148,15 +1297,20 @@
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
+          <t>Sem Categoria</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
           <t>19/09/2025 14:51</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>21/10/2025 19:51</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>21/10/2025 22:17</t>
         </is>
@@ -1179,15 +1333,20 @@
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
+          <t>Sem Categoria</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
           <t>19/09/2025 19:57</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>25/09/2025 23:16</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>21/10/2025 22:17</t>
         </is>
@@ -1210,15 +1369,20 @@
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
+          <t>Sem Categoria</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
           <t>19/09/2025 20:03</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>19/09/2025 20:44</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>21/10/2025 22:17</t>
         </is>
@@ -1241,15 +1405,20 @@
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
+          <t>Sem Categoria</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
           <t>19/09/2025 14:55</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>19/09/2025 20:22</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>21/10/2025 22:17</t>
         </is>
@@ -1272,15 +1441,20 @@
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr">
         <is>
+          <t>Sem Categoria</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
           <t>19/09/2025 20:43</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>19/09/2025 20:43</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>21/10/2025 22:17</t>
         </is>
@@ -1303,15 +1477,20 @@
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr">
         <is>
+          <t>Sem Categoria</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
           <t>19/09/2025 20:43</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>25/09/2025 23:08</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>21/10/2025 22:17</t>
         </is>
@@ -1334,15 +1513,20 @@
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr">
         <is>
+          <t>Sem Categoria</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
           <t>19/09/2025 20:43</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>25/09/2025 23:16</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>21/10/2025 22:17</t>
         </is>
@@ -1367,15 +1551,20 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
+          <t>Sem Categoria</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
           <t>21/10/2025 23:41</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>21/10/2025 23:41</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>21/10/2025 23:51</t>
         </is>
@@ -1400,15 +1589,20 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
+          <t>Sem Categoria</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
           <t>21/10/2025 23:42</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>21/10/2025 23:42</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>21/10/2025 23:51</t>
         </is>
@@ -1433,17 +1627,216 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
+          <t>Sem Categoria</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
           <t>21/10/2025 22:16</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>21/10/2025 22:17</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>23/10/2025 23:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>da</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>ID_16</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>cimento</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>29/10/2025 20:21</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>29/10/2025 20:21</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>29/10/2025 21:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>cimento 20kg</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>ID_7</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>25</v>
+      </c>
+      <c r="D20" t="n">
+        <v>406.9</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Sem Categoria</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:29</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>21/10/2025 22:56</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>29/10/2025 21:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>gugu</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>ID_14</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" t="n">
+        <v>12</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Sem Categoria</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>23/10/2025 23:59</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>23/10/2025 23:59</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>29/10/2025 21:23</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Categoria</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Sem Categoria</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>cimento</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>bucha</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>canos</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>parafusos</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>prego</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>maquinas</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>gugu</t>
         </is>
       </c>
     </row>

</xml_diff>